<commit_message>
ResNet in mxnet.gluon for deeplearning
</commit_message>
<xml_diff>
--- a/resnet-gluon/ResNetParam.xlsx
+++ b/resnet-gluon/ResNetParam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Input_data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mx.init.Normal(sigma=0.5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(224, 224)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,43 +92,43 @@
     <t>Epoch9</t>
   </si>
   <si>
+    <t>Learning1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning3</t>
+  </si>
+  <si>
+    <t>Learning4</t>
+  </si>
+  <si>
+    <t>Learning5</t>
+  </si>
+  <si>
+    <t>Learning6</t>
+  </si>
+  <si>
+    <t>Epoch0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sgd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(224, 224)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mx.init.Xavier()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>adam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Learning1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Learning2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Learning3</t>
-  </si>
-  <si>
-    <t>Learning4</t>
-  </si>
-  <si>
-    <t>Learning5</t>
-  </si>
-  <si>
-    <t>Learning6</t>
-  </si>
-  <si>
-    <t>Epoch0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sgd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(224, 224)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mx.init.Xavier()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -370,6 +366,120 @@
         <a:xfrm>
           <a:off x="5543550" y="3600449"/>
           <a:ext cx="2019500" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1867563</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>448235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8684559" y="3619500"/>
+          <a:ext cx="1867563" cy="448235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2323038</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>476251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10749644" y="3469822"/>
+          <a:ext cx="2317594" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>34637</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>403289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13161818" y="3532909"/>
+          <a:ext cx="1956955" cy="403289"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,9 +800,9 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="F19" sqref="F19"/>
+      <selection pane="topRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -700,29 +810,30 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="31.25" customWidth="1"/>
     <col min="6" max="6" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.375" customWidth="1"/>
+    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -731,22 +842,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -767,10 +878,10 @@
         <v>64</v>
       </c>
       <c r="G3" s="1">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -779,22 +890,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -806,19 +917,19 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -839,7 +950,7 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H6" s="1">
         <v>0.1</v>
@@ -874,7 +985,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
         <v>0.95342548076922995</v>
@@ -885,12 +996,14 @@
       <c r="E8" s="1">
         <v>0.95643028846153799</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>9.7956730769230699E-2</v>
+      </c>
       <c r="G8" s="1">
-        <v>9.8056000000000004E-2</v>
+        <v>0.92978766025641002</v>
       </c>
       <c r="H8" s="1">
-        <v>0.51492300000000002</v>
+        <v>0.72786458333333304</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,12 +1020,14 @@
       <c r="E9" s="1">
         <v>0.96654647435897401</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>9.8056891025640996E-2</v>
+      </c>
       <c r="G9" s="1">
-        <v>9.8056000000000004E-2</v>
+        <v>0.95342548076922995</v>
       </c>
       <c r="H9" s="1">
-        <v>0.75100100000000003</v>
+        <v>0.70222355769230704</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -929,10 +1044,14 @@
       <c r="E10" s="2">
         <v>0.96885016025641002</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="1">
+        <v>9.7856570512820498E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.97896634615384603</v>
+      </c>
       <c r="H10" s="1">
-        <v>0.80989500000000003</v>
+        <v>0.84745592948717896</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -949,16 +1068,20 @@
       <c r="E11" s="2">
         <v>0.97275641025641002</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1">
+        <v>9.7856570512820498E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.98978365384615297</v>
+      </c>
       <c r="H11" s="1">
-        <v>0.84064499999999998</v>
+        <v>0.903445512820512</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>0.97175480769230704</v>
@@ -969,16 +1092,20 @@
       <c r="E12" s="2">
         <v>0.97716346153846101</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1">
+        <v>9.7956730769230699E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.98988381410256399</v>
+      </c>
       <c r="H12" s="1">
-        <v>0.86227900000000002</v>
+        <v>0.94491185897435803</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>0.92067307692307598</v>
@@ -989,16 +1116,20 @@
       <c r="E13" s="2">
         <v>0.97996794871794801</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="1">
+        <v>9.7956730769230699E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.99228766025641002</v>
+      </c>
       <c r="H13" s="1">
-        <v>0.87279600000000002</v>
+        <v>0.94451121794871795</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
         <v>0.95602964743589702</v>
@@ -1009,16 +1140,20 @@
       <c r="E14" s="2">
         <v>0.98066907051282004</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1">
+        <v>9.8056891025640996E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.99158653846153799</v>
+      </c>
       <c r="H14" s="1">
-        <v>0.89052399999999998</v>
+        <v>0.96854967948717896</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>0.98237179487179405</v>
@@ -1029,16 +1164,20 @@
       <c r="E15" s="2">
         <v>0.97846554487179405</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1">
+        <v>9.7756410256410201E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.99008413461538403</v>
+      </c>
       <c r="H15" s="1">
-        <v>0.90104099999999998</v>
+        <v>0.92037259615384603</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
         <v>0.991085737179487</v>
@@ -1049,16 +1188,20 @@
       <c r="E16" s="2">
         <v>0.98417467948717896</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1">
+        <v>9.7956730769230699E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.98828125</v>
+      </c>
       <c r="H16" s="1">
-        <v>0.90805199999999997</v>
+        <v>0.96704727564102499</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
         <v>0.99078525641025605</v>
@@ -1069,10 +1212,14 @@
       <c r="E17" s="2">
         <v>0.98677884615384603</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1">
+        <v>9.8056891025640996E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.99208733974358898</v>
+      </c>
       <c r="H17" s="1">
-        <v>0.91366099999999995</v>
+        <v>0.89683493589743501</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>